<commit_message>
commit with new results
</commit_message>
<xml_diff>
--- a/test_si.xlsx
+++ b/test_si.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,6 @@
       <c r="A3" t="n">
         <v>13</v>
       </c>
-      <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
         <v>0.1857052532366953</v>
       </c>
@@ -527,6 +526,247 @@
       <c r="H3" t="inlineStr">
         <is>
           <t>['SKP1', 'KPNA4', 'ANAPC4', 'POLR2D', 'POLR2B', 'ANAPC11', 'POLE4', 'EDC3', 'RELB', 'NT5C2', 'PDE6H', 'PTPN6', 'TNFRSF10A']</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.2872303247797749</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0:00:15.920702</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2028611111111111</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.3715995384484387</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>['MAPK12', 'TRIM23', 'CIT', 'TNS1', 'PIK3C2A', 'RAF1', 'PPP3R1', 'MAPK1']</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>25</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1876826590545108</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0:00:16.956974</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0.16532</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.2100453181090215</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>['AURKA', 'NFKBIB', 'PI3', 'PIK3CB', 'AKT1', 'KIF22', 'EXOC2', 'PRKACB', 'PIK3C3', 'PLCG1', 'DLGAP5', 'RHOBTB1', 'NFKBIA', 'NFKB1', 'GABARAPL2', 'TLR3', 'RAC3', 'PPP3CA', 'SOS2', 'TNF', 'CHEK1', 'SYK', 'RPS6KB1', 'PPP1CB', 'PRKCI']</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.3888482498927541</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>0:00:15.162950</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0.4126000000000001</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.3650964997855081</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>['POLE2', 'POLR2H', 'POLR2I', 'NME3', 'GTF2H4']</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.2473947613832676</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0:00:15.366835</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0.185</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.3097895227665352</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>['RPS6KA2', 'MKKS', 'MAPK12', 'CDK16']</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.417886679229579</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0:00:15.682973</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0.5034285714285714</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.3323447870305865</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>['PSMC6', 'PSME2', 'UBA52', 'PSMA6', 'PPP2CB', 'NFKBIA', 'PPP2R5B']</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.3839870264497305</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0:00:15.047124</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0.3473928571428572</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.4205811957566039</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>['YWHAZ', 'INS', 'GAPDH', 'CDKN1B', 'AURKA', 'PIN1', 'NFKBIA']</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>20</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.2117678632919119</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0:00:16.964040</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1725666666666666</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.2509690599171571</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>['RALA', 'MAPK12', 'SOS2', 'HGF', 'NFKB1', 'PPP1CA', 'FGFR3', 'RAC1', 'TNS1', 'KIF22', 'PPP1CC', 'PPP2R1A', 'AURKA', 'STAG2', 'SOS1', 'PPP2R5B', 'DCN', 'DLGAP5', 'SIRT1', 'PPP3CA']</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.3978440954282857</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0:00:16.238540</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.3456881908565715</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>['ANAPC7', 'UBE2V2', 'SKP1', 'NFKB1', 'FBXL15']</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>8</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.4865680695869101</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0:00:16.228390</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0.6094444444444443</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.3636916947293759</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>['KALRN', 'PIK3R2', 'GNA11', 'GNRHR', 'GAST', 'KISS1R', 'GNG4', 'GNG7']</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="n">
+        <v>0.05330980403894163</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0:00:02.387701</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0.04619696969696969</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.06042263838091356</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>['FCGR3B', 'CLPS', 'LILRB3', 'TP53', 'PDE5A', 'IL3RA', 'CD79A', 'CHP2', 'PIK3CD', 'TNF', 'C1DP3']</t>
         </is>
       </c>
     </row>

</xml_diff>